<commit_message>
Data update and variable toggles for gaze delay
</commit_message>
<xml_diff>
--- a/Grid_Data.xlsx
+++ b/Grid_Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="215">
   <si>
     <t>TABLE</t>
   </si>
@@ -429,6 +429,246 @@
   </si>
   <si>
     <t>12,9</t>
+  </si>
+  <si>
+    <t>9X15</t>
+  </si>
+  <si>
+    <t>9X17</t>
+  </si>
+  <si>
+    <t>9,4</t>
+  </si>
+  <si>
+    <t>6,14</t>
+  </si>
+  <si>
+    <t>4,12</t>
+  </si>
+  <si>
+    <t>9,11</t>
+  </si>
+  <si>
+    <t>4,15</t>
+  </si>
+  <si>
+    <t>5,11</t>
+  </si>
+  <si>
+    <t>2,14</t>
+  </si>
+  <si>
+    <t>1,15</t>
+  </si>
+  <si>
+    <t>8,11</t>
+  </si>
+  <si>
+    <t>2,12</t>
+  </si>
+  <si>
+    <t>9,19</t>
+  </si>
+  <si>
+    <t>8,18</t>
+  </si>
+  <si>
+    <t>3,14</t>
+  </si>
+  <si>
+    <t>3,11</t>
+  </si>
+  <si>
+    <t>3,15</t>
+  </si>
+  <si>
+    <t>2,15</t>
+  </si>
+  <si>
+    <t>1,12</t>
+  </si>
+  <si>
+    <t>4,14</t>
+  </si>
+  <si>
+    <t>4,13</t>
+  </si>
+  <si>
+    <t>7,12</t>
+  </si>
+  <si>
+    <t>7,14</t>
+  </si>
+  <si>
+    <t>7,15</t>
+  </si>
+  <si>
+    <t>3,8</t>
+  </si>
+  <si>
+    <t>9,13</t>
+  </si>
+  <si>
+    <t>9,14</t>
+  </si>
+  <si>
+    <t>1,14</t>
+  </si>
+  <si>
+    <t>8,14</t>
+  </si>
+  <si>
+    <t>8,15</t>
+  </si>
+  <si>
+    <t>7,17</t>
+  </si>
+  <si>
+    <t>8,16</t>
+  </si>
+  <si>
+    <t>9,16</t>
+  </si>
+  <si>
+    <t>8,17</t>
+  </si>
+  <si>
+    <t>6,16</t>
+  </si>
+  <si>
+    <t>4,17</t>
+  </si>
+  <si>
+    <t>8,10</t>
+  </si>
+  <si>
+    <t>4,16</t>
+  </si>
+  <si>
+    <t>6,8</t>
+  </si>
+  <si>
+    <t>5,14</t>
+  </si>
+  <si>
+    <t>5,16</t>
+  </si>
+  <si>
+    <t>1,17</t>
+  </si>
+  <si>
+    <t>9,15</t>
+  </si>
+  <si>
+    <t>3,17</t>
+  </si>
+  <si>
+    <t>5,9</t>
+  </si>
+  <si>
+    <t>6,15</t>
+  </si>
+  <si>
+    <t>3,16</t>
+  </si>
+  <si>
+    <t>6,13</t>
+  </si>
+  <si>
+    <t>1,16</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>9X19</t>
+  </si>
+  <si>
+    <t>5,18</t>
+  </si>
+  <si>
+    <t>9,18</t>
+  </si>
+  <si>
+    <t>3,18</t>
+  </si>
+  <si>
+    <t>5,19</t>
+  </si>
+  <si>
+    <t>1,19</t>
+  </si>
+  <si>
+    <t>2,18</t>
+  </si>
+  <si>
+    <t>2,16</t>
+  </si>
+  <si>
+    <t>6,19</t>
+  </si>
+  <si>
+    <t>7,18</t>
+  </si>
+  <si>
+    <t>5,12</t>
+  </si>
+  <si>
+    <t>4,19</t>
+  </si>
+  <si>
+    <t>2,19</t>
+  </si>
+  <si>
+    <t>3,19</t>
+  </si>
+  <si>
+    <t>7,19</t>
+  </si>
+  <si>
+    <t>9X23</t>
+  </si>
+  <si>
+    <t>2,21</t>
+  </si>
+  <si>
+    <t>4,20</t>
+  </si>
+  <si>
+    <t>6,23</t>
+  </si>
+  <si>
+    <t>8,22</t>
+  </si>
+  <si>
+    <t>7,22</t>
+  </si>
+  <si>
+    <t>2,23</t>
+  </si>
+  <si>
+    <t>1,23</t>
+  </si>
+  <si>
+    <t>6,22</t>
+  </si>
+  <si>
+    <t>9,22</t>
+  </si>
+  <si>
+    <t>9,17</t>
+  </si>
+  <si>
+    <t>3,22</t>
+  </si>
+  <si>
+    <t>5,21</t>
+  </si>
+  <si>
+    <t>6,21</t>
+  </si>
+  <si>
+    <t>1,20</t>
   </si>
 </sst>
 </file>
@@ -783,15 +1023,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U54"/>
+  <dimension ref="A2:BD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="AP30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AW52" sqref="AW52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -804,8 +1044,23 @@
       <c r="P2" t="s">
         <v>98</v>
       </c>
+      <c r="W2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>184</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -824,8 +1079,38 @@
       <c r="S3" t="s">
         <v>16</v>
       </c>
+      <c r="W3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -880,8 +1165,98 @@
       <c r="U4" t="s">
         <v>31</v>
       </c>
+      <c r="W4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -939,8 +1314,86 @@
       <c r="U5" s="1">
         <v>0</v>
       </c>
+      <c r="W5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR5" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AS5" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AT5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AV5" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AW5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="1"/>
+      <c r="BC5" s="1"/>
+      <c r="BD5" s="1"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -995,8 +1448,86 @@
       <c r="U6" s="1">
         <v>1</v>
       </c>
+      <c r="W6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AS6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AT6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU6" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AV6" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AW6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="1"/>
+      <c r="BC6" s="1"/>
+      <c r="BD6" s="1"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1051,8 +1582,86 @@
       <c r="U7" s="1">
         <v>1</v>
       </c>
+      <c r="W7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU7" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AV7" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AW7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="1"/>
+      <c r="BC7" s="1"/>
+      <c r="BD7" s="1"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1107,8 +1716,86 @@
       <c r="U8" s="1">
         <v>1</v>
       </c>
+      <c r="W8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR8" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AS8" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AT8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AV8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AW8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="1"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1163,8 +1850,86 @@
       <c r="U9" s="1">
         <v>0</v>
       </c>
+      <c r="W9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AM9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AP9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR9" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AS9" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="1"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1219,8 +1984,86 @@
       <c r="U10" s="1">
         <v>1</v>
       </c>
+      <c r="W10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AM10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AV10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AW10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1275,8 +2118,86 @@
       <c r="U11" s="1">
         <v>1</v>
       </c>
+      <c r="W11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AS11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1331,8 +2252,86 @@
       <c r="U12" s="1">
         <v>1</v>
       </c>
+      <c r="W12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AS12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AV12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="1"/>
+      <c r="BC12" s="1"/>
+      <c r="BD12" s="1"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1387,8 +2386,86 @@
       <c r="U13" s="1">
         <v>1</v>
       </c>
+      <c r="W13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AM13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN13" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AO13" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AP13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR13" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AS13" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AT13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AV13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AW13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="1"/>
+      <c r="BA13" s="1"/>
+      <c r="BB13" s="1"/>
+      <c r="BC13" s="1"/>
+      <c r="BD13" s="1"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1443,8 +2520,86 @@
       <c r="U14" s="1">
         <v>1</v>
       </c>
+      <c r="W14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AL14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AP14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AS14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AT14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU14" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV14" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AW14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
+      <c r="BA14" s="1"/>
+      <c r="BB14" s="1"/>
+      <c r="BC14" s="1"/>
+      <c r="BD14" s="1"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
@@ -1454,7 +2609,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1">
-        <f t="shared" ref="E15:U15" si="0">SUM(G5:G14)/10</f>
+        <f t="shared" ref="G15:U15" si="0">SUM(G5:G14)/10</f>
         <v>0.4</v>
       </c>
       <c r="H15" s="1"/>
@@ -1483,8 +2638,67 @@
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1">
+        <f t="shared" ref="Y15:AB15" si="1">SUM(Y5:Y14)/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1">
+        <f t="shared" ref="AB15" si="2">SUM(AB5:AB14)/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1">
+        <f>SUM(AF5:AF14)/10</f>
+        <v>1</v>
+      </c>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1">
+        <f>SUM(AI5:AI14)/10</f>
+        <v>1</v>
+      </c>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1">
+        <f t="shared" ref="AM15:AP15" si="3">SUM(AM5:AM14)/10</f>
+        <v>1</v>
+      </c>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1">
+        <f t="shared" ref="AP15" si="4">SUM(AP5:AP14)/10</f>
+        <v>1</v>
+      </c>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1">
+        <f t="shared" ref="AT15:AW15" si="5">SUM(AT5:AT14)/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1">
+        <f t="shared" ref="BA15:BD15" si="6">SUM(BA5:BA14)/10</f>
+        <v>0</v>
+      </c>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BD15" s="1">
+        <f t="shared" ref="BD15" si="7">SUM(BD5:BD14)/10</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -1503,8 +2717,44 @@
       <c r="S16" t="s">
         <v>16</v>
       </c>
+      <c r="W16" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK16" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB16" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1559,8 +2809,98 @@
       <c r="U17" t="s">
         <v>31</v>
       </c>
+      <c r="W17" t="s">
+        <v>3</v>
+      </c>
+      <c r="X17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC17" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD17" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1618,8 +2958,86 @@
       <c r="U18" s="1">
         <v>1</v>
       </c>
+      <c r="W18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AL18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AM18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AS18" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AT18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU18" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AV18" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY18" s="1"/>
+      <c r="AZ18" s="1"/>
+      <c r="BA18" s="1"/>
+      <c r="BB18" s="1"/>
+      <c r="BC18" s="1"/>
+      <c r="BD18" s="1"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B19" s="1" t="s">
         <v>32</v>
       </c>
@@ -1674,8 +3092,86 @@
       <c r="U19" s="1">
         <v>1</v>
       </c>
+      <c r="W19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AI19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AV19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AW19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY19" s="1"/>
+      <c r="AZ19" s="1"/>
+      <c r="BA19" s="1"/>
+      <c r="BB19" s="1"/>
+      <c r="BC19" s="1"/>
+      <c r="BD19" s="1"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1730,8 +3226,86 @@
       <c r="U20" s="1">
         <v>1</v>
       </c>
+      <c r="W20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH20" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AO20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AT20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY20" s="1"/>
+      <c r="AZ20" s="1"/>
+      <c r="BA20" s="1"/>
+      <c r="BB20" s="1"/>
+      <c r="BC20" s="1"/>
+      <c r="BD20" s="1"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B21" s="1" t="s">
         <v>51</v>
       </c>
@@ -1786,8 +3360,86 @@
       <c r="U21" s="1">
         <v>1</v>
       </c>
+      <c r="W21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AM21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AO21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AP21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AS21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AT21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AV21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AW21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY21" s="1"/>
+      <c r="AZ21" s="1"/>
+      <c r="BA21" s="1"/>
+      <c r="BB21" s="1"/>
+      <c r="BC21" s="1"/>
+      <c r="BD21" s="1"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
@@ -1842,8 +3494,86 @@
       <c r="U22" s="1">
         <v>1</v>
       </c>
+      <c r="W22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AI22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AL22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AT22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU22" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AV22" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AW22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY22" s="1"/>
+      <c r="AZ22" s="1"/>
+      <c r="BA22" s="1"/>
+      <c r="BB22" s="1"/>
+      <c r="BC22" s="1"/>
+      <c r="BD22" s="1"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B23" s="1" t="s">
         <v>34</v>
       </c>
@@ -1898,8 +3628,86 @@
       <c r="U23" s="1">
         <v>1</v>
       </c>
+      <c r="W23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AH23" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AL23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AM23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN23" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AO23" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AV23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY23" s="1"/>
+      <c r="AZ23" s="1"/>
+      <c r="BA23" s="1"/>
+      <c r="BB23" s="1"/>
+      <c r="BC23" s="1"/>
+      <c r="BD23" s="1"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1954,8 +3762,86 @@
       <c r="U24" s="1">
         <v>1</v>
       </c>
+      <c r="W24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK24" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AL24" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AM24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN24" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AO24" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AP24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR24" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AS24" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AT24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU24" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AV24" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY24" s="1"/>
+      <c r="AZ24" s="1"/>
+      <c r="BA24" s="1"/>
+      <c r="BB24" s="1"/>
+      <c r="BC24" s="1"/>
+      <c r="BD24" s="1"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
@@ -2010,8 +3896,86 @@
       <c r="U25" s="1">
         <v>1</v>
       </c>
+      <c r="W25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE25" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AS25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AT25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AV25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AW25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY25" s="1"/>
+      <c r="AZ25" s="1"/>
+      <c r="BA25" s="1"/>
+      <c r="BB25" s="1"/>
+      <c r="BC25" s="1"/>
+      <c r="BD25" s="1"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B26" s="1" t="s">
         <v>40</v>
       </c>
@@ -2066,8 +4030,86 @@
       <c r="U26" s="1">
         <v>1</v>
       </c>
+      <c r="W26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AL26" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AM26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AO26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AP26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU26" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AV26" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY26" s="1"/>
+      <c r="AZ26" s="1"/>
+      <c r="BA26" s="1"/>
+      <c r="BB26" s="1"/>
+      <c r="BC26" s="1"/>
+      <c r="BD26" s="1"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2122,8 +4164,86 @@
       <c r="U27" s="1">
         <v>1</v>
       </c>
+      <c r="W27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AE27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK27" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AL27" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AM27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AS27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AT27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AV27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AW27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY27" s="1"/>
+      <c r="AZ27" s="1"/>
+      <c r="BA27" s="1"/>
+      <c r="BB27" s="1"/>
+      <c r="BC27" s="1"/>
+      <c r="BD27" s="1"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.45">
       <c r="D28" s="1">
         <f>SUM(D18:D27)/10</f>
         <v>1</v>
@@ -2148,8 +4268,47 @@
         <f>SUM(U18:U27)/10</f>
         <v>1</v>
       </c>
+      <c r="Y28" s="1">
+        <f>SUM(Y18:Y27)/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="AB28" s="1">
+        <f>SUM(AB18:AB27)/10</f>
+        <v>1</v>
+      </c>
+      <c r="AF28" s="1">
+        <f>SUM(AF18:AF27)/10</f>
+        <v>1</v>
+      </c>
+      <c r="AI28" s="1">
+        <f>SUM(AI18:AI27)/10</f>
+        <v>1</v>
+      </c>
+      <c r="AM28" s="1">
+        <f>SUM(AM18:AM27)/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="AP28" s="1">
+        <f>SUM(AP18:AP27)/10</f>
+        <v>0.9</v>
+      </c>
+      <c r="AT28" s="1">
+        <f>SUM(AT18:AT27)/10</f>
+        <v>1</v>
+      </c>
+      <c r="AW28" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="BA28" s="1">
+        <f>SUM(BA18:BA27)/10</f>
+        <v>0</v>
+      </c>
+      <c r="BD28" s="1">
+        <f>SUM(BD18:BD27)/10</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>15</v>
       </c>
@@ -2168,8 +4327,44 @@
       <c r="S29" t="s">
         <v>16</v>
       </c>
+      <c r="W29" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN29" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR29" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU29" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY29" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB29" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -2224,8 +4419,98 @@
       <c r="U30" t="s">
         <v>31</v>
       </c>
+      <c r="W30" t="s">
+        <v>3</v>
+      </c>
+      <c r="X30" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM30" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN30" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP30" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR30" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT30" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU30" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW30" t="s">
+        <v>31</v>
+      </c>
+      <c r="AY30" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ30" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA30" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB30" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC30" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD30" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2283,8 +4568,86 @@
       <c r="U31" s="1">
         <v>1</v>
       </c>
+      <c r="W31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="X31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR31" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AS31" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AV31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY31" s="1"/>
+      <c r="AZ31" s="1"/>
+      <c r="BA31" s="1"/>
+      <c r="BB31" s="1"/>
+      <c r="BC31" s="1"/>
+      <c r="BD31" s="1"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B32" s="1" t="s">
         <v>22</v>
       </c>
@@ -2339,8 +4702,86 @@
       <c r="U32" s="1">
         <v>0</v>
       </c>
+      <c r="W32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y32" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD32" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE32" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK32" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL32" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN32" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AO32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AP32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR32" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AS32" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AT32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AV32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AW32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY32" s="1"/>
+      <c r="AZ32" s="1"/>
+      <c r="BA32" s="1"/>
+      <c r="BB32" s="1"/>
+      <c r="BC32" s="1"/>
+      <c r="BD32" s="1"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
@@ -2395,8 +4836,86 @@
       <c r="U33" s="1">
         <v>1</v>
       </c>
+      <c r="W33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="X33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK33" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL33" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AM33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN33" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AO33" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AP33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AW33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY33" s="1"/>
+      <c r="AZ33" s="1"/>
+      <c r="BA33" s="1"/>
+      <c r="BB33" s="1"/>
+      <c r="BC33" s="1"/>
+      <c r="BD33" s="1"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B34" s="1" t="s">
         <v>20</v>
       </c>
@@ -2451,8 +4970,86 @@
       <c r="U34" s="1">
         <v>0</v>
       </c>
+      <c r="W34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="X34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL34" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AM34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR34" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AS34" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AT34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY34" s="1"/>
+      <c r="AZ34" s="1"/>
+      <c r="BA34" s="1"/>
+      <c r="BB34" s="1"/>
+      <c r="BC34" s="1"/>
+      <c r="BD34" s="1"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B35" s="1" t="s">
         <v>50</v>
       </c>
@@ -2507,8 +5104,86 @@
       <c r="U35" s="1">
         <v>1</v>
       </c>
+      <c r="W35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="X35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y35" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE35" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AF35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG35" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AH35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AV35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY35" s="1"/>
+      <c r="AZ35" s="1"/>
+      <c r="BA35" s="1"/>
+      <c r="BB35" s="1"/>
+      <c r="BC35" s="1"/>
+      <c r="BD35" s="1"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B36" s="1" t="s">
         <v>26</v>
       </c>
@@ -2563,8 +5238,86 @@
       <c r="U36" s="1">
         <v>1</v>
       </c>
+      <c r="W36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y36" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB36" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF36" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG36" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH36" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT36" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU36" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AV36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY36" s="1"/>
+      <c r="AZ36" s="1"/>
+      <c r="BA36" s="1"/>
+      <c r="BB36" s="1"/>
+      <c r="BC36" s="1"/>
+      <c r="BD36" s="1"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B37" s="1" t="s">
         <v>61</v>
       </c>
@@ -2619,8 +5372,86 @@
       <c r="U37" s="1">
         <v>1</v>
       </c>
+      <c r="W37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="X37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y37" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD37" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE37" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AL37" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AM37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN37" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AO37" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AP37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR37" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AS37" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AT37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU37" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AV37" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AW37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY37" s="1"/>
+      <c r="AZ37" s="1"/>
+      <c r="BA37" s="1"/>
+      <c r="BB37" s="1"/>
+      <c r="BC37" s="1"/>
+      <c r="BD37" s="1"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B38" s="1" t="s">
         <v>27</v>
       </c>
@@ -2675,8 +5506,86 @@
       <c r="U38" s="1">
         <v>0</v>
       </c>
+      <c r="W38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE38" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN38" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AO38" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AP38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AS38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU38" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AV38" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AW38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY38" s="1"/>
+      <c r="AZ38" s="1"/>
+      <c r="BA38" s="1"/>
+      <c r="BB38" s="1"/>
+      <c r="BC38" s="1"/>
+      <c r="BD38" s="1"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B39" s="1" t="s">
         <v>14</v>
       </c>
@@ -2731,8 +5640,86 @@
       <c r="U39" s="1">
         <v>1</v>
       </c>
+      <c r="W39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y39" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA39" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AE39" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG39" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AH39" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AI39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK39" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AL39" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AM39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AT39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU39" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AV39" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AW39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY39" s="1"/>
+      <c r="AZ39" s="1"/>
+      <c r="BA39" s="1"/>
+      <c r="BB39" s="1"/>
+      <c r="BC39" s="1"/>
+      <c r="BD39" s="1"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B40" s="1" t="s">
         <v>30</v>
       </c>
@@ -2787,8 +5774,86 @@
       <c r="U40" s="1">
         <v>0</v>
       </c>
+      <c r="W40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="X40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y40" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD40" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE40" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR40" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AS40" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AT40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AV40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AW40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY40" s="1"/>
+      <c r="AZ40" s="1"/>
+      <c r="BA40" s="1"/>
+      <c r="BB40" s="1"/>
+      <c r="BC40" s="1"/>
+      <c r="BD40" s="1"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1">
@@ -2825,8 +5890,68 @@
         <f>SUM(U31:U40)/10</f>
         <v>0.6</v>
       </c>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1">
+        <f>SUM(Y31:Y40)/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="1">
+        <f>SUM(AB31:AB40)/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="1"/>
+      <c r="AF41" s="1">
+        <f>SUM(AF31:AF40)/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="AG41" s="1"/>
+      <c r="AH41" s="1"/>
+      <c r="AI41" s="1">
+        <f>SUM(AI31:AI40)/10</f>
+        <v>0.3</v>
+      </c>
+      <c r="AK41" s="1"/>
+      <c r="AL41" s="1"/>
+      <c r="AM41" s="1">
+        <f>SUM(AM31:AM40)/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="AN41" s="1"/>
+      <c r="AO41" s="1"/>
+      <c r="AP41" s="1">
+        <f>SUM(AP31:AP40)/10</f>
+        <v>0.6</v>
+      </c>
+      <c r="AR41" s="1"/>
+      <c r="AS41" s="1"/>
+      <c r="AT41" s="1">
+        <f>SUM(AT31:AT40)/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="AU41" s="1"/>
+      <c r="AV41" s="1"/>
+      <c r="AW41" s="1">
+        <f>SUM(AW31:AW40)/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="AY41" s="1"/>
+      <c r="AZ41" s="1"/>
+      <c r="BA41" s="1">
+        <f>SUM(BA31:BA40)/10</f>
+        <v>0</v>
+      </c>
+      <c r="BB41" s="1"/>
+      <c r="BC41" s="1"/>
+      <c r="BD41" s="1">
+        <f>SUM(BD31:BD40)/10</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>15</v>
       </c>
@@ -2845,8 +5970,44 @@
       <c r="S42" t="s">
         <v>16</v>
       </c>
+      <c r="W42" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD42" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK42" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN42" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR42" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU42" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY42" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB42" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
         <v>3</v>
       </c>
@@ -2901,8 +6062,98 @@
       <c r="U43" t="s">
         <v>31</v>
       </c>
+      <c r="W43" t="s">
+        <v>3</v>
+      </c>
+      <c r="X43" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH43" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL43" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM43" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO43" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP43" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS43" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT43" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV43" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW43" t="s">
+        <v>31</v>
+      </c>
+      <c r="AY43" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ43" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA43" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB43" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC43" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD43" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -2960,8 +6211,86 @@
       <c r="U44" s="1">
         <v>1</v>
       </c>
+      <c r="W44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE44" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL44" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AO44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR44" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AS44" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AT44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU44" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AV44" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AW44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY44" s="1"/>
+      <c r="AZ44" s="1"/>
+      <c r="BA44" s="1"/>
+      <c r="BB44" s="1"/>
+      <c r="BC44" s="1"/>
+      <c r="BD44" s="1"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B45" s="1" t="s">
         <v>32</v>
       </c>
@@ -3016,8 +6345,86 @@
       <c r="U45" s="1">
         <v>1</v>
       </c>
+      <c r="W45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="X45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y45" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD45" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE45" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG45" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH45" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AI45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK45" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AL45" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN45" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AO45" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AP45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR45" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AS45" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AT45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AV45" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AW45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY45" s="1"/>
+      <c r="AZ45" s="1"/>
+      <c r="BA45" s="1"/>
+      <c r="BB45" s="1"/>
+      <c r="BC45" s="1"/>
+      <c r="BD45" s="1"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B46" s="1" t="s">
         <v>5</v>
       </c>
@@ -3072,8 +6479,86 @@
       <c r="U46" s="1">
         <v>1</v>
       </c>
+      <c r="W46" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="X46" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y46" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD46" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG46" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH46" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AI46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR46" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AS46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU46" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AV46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AW46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY46" s="1"/>
+      <c r="AZ46" s="1"/>
+      <c r="BA46" s="1"/>
+      <c r="BB46" s="1"/>
+      <c r="BC46" s="1"/>
+      <c r="BD46" s="1"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B47" s="1" t="s">
         <v>42</v>
       </c>
@@ -3128,8 +6613,86 @@
       <c r="U47" s="1">
         <v>0</v>
       </c>
+      <c r="W47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="X47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y47" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD47" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE47" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AH47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AS47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU47" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AV47" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AW47" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY47" s="1"/>
+      <c r="AZ47" s="1"/>
+      <c r="BA47" s="1"/>
+      <c r="BB47" s="1"/>
+      <c r="BC47" s="1"/>
+      <c r="BD47" s="1"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:56" x14ac:dyDescent="0.45">
       <c r="B48" s="1" t="s">
         <v>40</v>
       </c>
@@ -3184,8 +6747,86 @@
       <c r="U48" s="1">
         <v>1</v>
       </c>
+      <c r="W48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y48" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA48" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE48" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG48" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH48" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI48" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN48" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AO48" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AP48" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR48" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AS48" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AT48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU48" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AV48" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AW48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY48" s="1"/>
+      <c r="AZ48" s="1"/>
+      <c r="BA48" s="1"/>
+      <c r="BB48" s="1"/>
+      <c r="BC48" s="1"/>
+      <c r="BD48" s="1"/>
     </row>
-    <row r="49" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:56" x14ac:dyDescent="0.45">
       <c r="B49" s="1" t="s">
         <v>67</v>
       </c>
@@ -3240,8 +6881,86 @@
       <c r="U49" s="1">
         <v>1</v>
       </c>
+      <c r="W49" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="X49" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y49" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD49" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE49" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AF49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM49" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP49" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT49" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU49" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AV49" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AW49" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY49" s="1"/>
+      <c r="AZ49" s="1"/>
+      <c r="BA49" s="1"/>
+      <c r="BB49" s="1"/>
+      <c r="BC49" s="1"/>
+      <c r="BD49" s="1"/>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:56" x14ac:dyDescent="0.45">
       <c r="B50" s="1" t="s">
         <v>51</v>
       </c>
@@ -3296,8 +7015,86 @@
       <c r="U50" s="1">
         <v>1</v>
       </c>
+      <c r="W50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y50" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA50" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE50" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL50" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN50" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AO50" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AP50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AT50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY50" s="1"/>
+      <c r="AZ50" s="1"/>
+      <c r="BA50" s="1"/>
+      <c r="BB50" s="1"/>
+      <c r="BC50" s="1"/>
+      <c r="BD50" s="1"/>
     </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:56" x14ac:dyDescent="0.45">
       <c r="B51" s="1" t="s">
         <v>8</v>
       </c>
@@ -3352,8 +7149,86 @@
       <c r="U51" s="1">
         <v>1</v>
       </c>
+      <c r="W51" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="X51" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y51" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB51" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF51" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI51" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK51" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL51" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AM51" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN51" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO51" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP51" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR51" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AS51" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AT51" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AV51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW51" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY51" s="1"/>
+      <c r="AZ51" s="1"/>
+      <c r="BA51" s="1"/>
+      <c r="BB51" s="1"/>
+      <c r="BC51" s="1"/>
+      <c r="BD51" s="1"/>
     </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:56" x14ac:dyDescent="0.45">
       <c r="B52" s="1" t="s">
         <v>56</v>
       </c>
@@ -3408,8 +7283,86 @@
       <c r="U52" s="1">
         <v>1</v>
       </c>
+      <c r="W52" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="X52" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y52" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z52" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA52" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE52" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AF52" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM52" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN52" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO52" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR52" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AT52" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY52" s="1"/>
+      <c r="AZ52" s="1"/>
+      <c r="BA52" s="1"/>
+      <c r="BB52" s="1"/>
+      <c r="BC52" s="1"/>
+      <c r="BD52" s="1"/>
     </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:56" x14ac:dyDescent="0.45">
       <c r="B53" s="1" t="s">
         <v>70</v>
       </c>
@@ -3464,8 +7417,86 @@
       <c r="U53" s="1">
         <v>1</v>
       </c>
+      <c r="W53" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="X53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y53" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA53" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB53" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD53" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE53" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH53" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="AI53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK53" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN53" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AO53" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AP53" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR53" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AS53" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AT53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV53" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AW53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY53" s="1"/>
+      <c r="AZ53" s="1"/>
+      <c r="BA53" s="1"/>
+      <c r="BB53" s="1"/>
+      <c r="BC53" s="1"/>
+      <c r="BD53" s="1"/>
     </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:56" x14ac:dyDescent="0.45">
       <c r="D54" s="1">
         <f>SUM(D44:D53)/10</f>
         <v>0.7</v>
@@ -3489,6 +7520,47 @@
       <c r="U54" s="1">
         <f>SUM(U44:U53)/10</f>
         <v>0.9</v>
+      </c>
+      <c r="Y54" s="1">
+        <f>SUM(Y44:Y53)/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="AB54" s="1">
+        <f>SUM(AB44:AB53)/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="AF54" s="1">
+        <f>SUM(AF44:AF53)/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="AG54" s="1"/>
+      <c r="AI54" s="1">
+        <f>SUM(AI44:AI53)/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="AM54" s="1">
+        <f>SUM(AM44:AM53)/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="AP54" s="1">
+        <f>SUM(AP44:AP53)/10</f>
+        <v>1</v>
+      </c>
+      <c r="AT54" s="1">
+        <f>SUM(AT44:AT53)/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="AW54" s="1">
+        <f>SUM(AW44:AW53)/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="BA54" s="1">
+        <f>SUM(BA44:BA53)/10</f>
+        <v>0</v>
+      </c>
+      <c r="BD54" s="1">
+        <f>SUM(BD44:BD53)/10</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>